<commit_message>
Export user data to excel file.
</commit_message>
<xml_diff>
--- a/assets/excel/PEBRA_Data_template.xlsx
+++ b/assets/excel/PEBRA_Data_template.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Dev/PEBRApp/assets/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Dev/repos/PEBRApp/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3B30F2-13EB-BB46-9654-2992F6D596AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A47869E-F6B4-714A-952A-BF3CF7001717}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="33340" windowHeight="22800" xr2:uid="{46424636-BBCA-2C45-853D-B40C826B6618}"/>
+    <workbookView xWindow="780" yWindow="960" windowWidth="43600" windowHeight="24960" xr2:uid="{46424636-BBCA-2C45-853D-B40C826B6618}"/>
   </bookViews>
   <sheets>
-    <sheet name="Patient" sheetId="1" r:id="rId1"/>
-    <sheet name="Viral Load" sheetId="2" r:id="rId2"/>
-    <sheet name="Preference Assessment" sheetId="3" r:id="rId3"/>
-    <sheet name="ART Refill" sheetId="4" r:id="rId4"/>
+    <sheet name="User Data" sheetId="5" r:id="rId1"/>
+    <sheet name="Patient" sheetId="1" r:id="rId2"/>
+    <sheet name="Viral Load" sheetId="2" r:id="rId3"/>
+    <sheet name="Preference Assessment" sheetId="3" r:id="rId4"/>
+    <sheet name="ART Refill" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ART Refill</t>
   </si>
@@ -46,6 +47,9 @@
   </si>
   <si>
     <t>Patient</t>
+  </si>
+  <si>
+    <t>User Data</t>
   </si>
 </sst>
 </file>
@@ -402,10 +406,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F14C1D3F-DADE-7948-96C4-CAE9F01E0419}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F39E4D3-A1E0-134D-B622-AE1D67844ECA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -419,7 +441,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15AFD532-25CD-4148-BDDB-ED6AB75CCFF4}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -438,7 +460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B32EA6C-2439-4446-BC47-7B3F83C87FCB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -456,7 +478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9BE023-1C31-614C-918B-D51772EA5AE2}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Export support option done data to excel file.
</commit_message>
<xml_diff>
--- a/assets/excel/PEBRA_Data_template.xlsx
+++ b/assets/excel/PEBRA_Data_template.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Dev/repos/PEBRApp/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A47869E-F6B4-714A-952A-BF3CF7001717}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801C8149-59BC-8740-B2BD-5AEEDCFFDAA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="43600" windowHeight="24960" xr2:uid="{46424636-BBCA-2C45-853D-B40C826B6618}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{46424636-BBCA-2C45-853D-B40C826B6618}"/>
   </bookViews>
   <sheets>
     <sheet name="User Data" sheetId="5" r:id="rId1"/>
     <sheet name="Patient" sheetId="1" r:id="rId2"/>
     <sheet name="Viral Load" sheetId="2" r:id="rId3"/>
     <sheet name="Preference Assessment" sheetId="3" r:id="rId4"/>
-    <sheet name="ART Refill" sheetId="4" r:id="rId5"/>
+    <sheet name="Support Option Done" sheetId="6" r:id="rId5"/>
+    <sheet name="ART Refill" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>ART Refill</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t>User Data</t>
+  </si>
+  <si>
+    <t>Support Option Done</t>
   </si>
 </sst>
 </file>
@@ -479,6 +483,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D14B88-3B73-C34A-86A7-617B985326A4}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9BE023-1C31-614C-918B-D51772EA5AE2}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changed 'patient' to 'participant' in UI.
</commit_message>
<xml_diff>
--- a/assets/excel/PEBRA_Data_template.xlsx
+++ b/assets/excel/PEBRA_Data_template.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Dev/repos/PEBRApp/assets/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801C8149-59BC-8740-B2BD-5AEEDCFFDAA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E01D6BC0-274D-3948-805E-AF42BD4F7986}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{46424636-BBCA-2C45-853D-B40C826B6618}"/>
   </bookViews>
   <sheets>
     <sheet name="User Data" sheetId="5" r:id="rId1"/>
-    <sheet name="Patient" sheetId="1" r:id="rId2"/>
+    <sheet name="Participant" sheetId="1" r:id="rId2"/>
     <sheet name="Viral Load" sheetId="2" r:id="rId3"/>
     <sheet name="Preference Assessment" sheetId="3" r:id="rId4"/>
     <sheet name="Support Option Done" sheetId="6" r:id="rId5"/>
@@ -47,13 +47,13 @@
     <t>Viral Load</t>
   </si>
   <si>
-    <t>Patient</t>
-  </si>
-  <si>
     <t>User Data</t>
   </si>
   <si>
     <t>Support Option Done</t>
+  </si>
+  <si>
+    <t>Participant</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -437,7 +437,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -492,7 +492,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>